<commit_message>
agregue pame.html confirmacion de pedidos
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -440,42 +440,42 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1739052234610</v>
+        <v>1739053700635</v>
       </c>
       <c r="B2" t="str">
         <v>Caipirinha</v>
       </c>
       <c r="C2" t="str">
-        <v>2 litro(s)</v>
+        <v>1 litro(s)</v>
       </c>
       <c r="D2" t="str">
-        <v>Efectivo</v>
+        <v>Transferencia</v>
       </c>
       <c r="E2" t="str">
-        <v>2</v>
+        <v>manu</v>
       </c>
       <c r="F2" t="str">
         <v>595971224560</v>
       </c>
       <c r="G2" t="str">
-        <v>8/2/2025, 19:04:00</v>
+        <v>8/2/2025, 19:28:24</v>
       </c>
       <c r="H2" t="str">
         <v>Terminado</v>
       </c>
       <c r="I2" t="str">
-        <v>8/2/2025, 19:04:19</v>
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>8/2/2025, 19:04:53</v>
+        <v>8/2/2025, 19:35:06</v>
       </c>
       <c r="K2" t="str">
-        <v>Nico</v>
+        <v>Marcos</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1739052247441</v>
+        <v>1739053945837</v>
       </c>
       <c r="B3" t="str">
         <v>Caipirinha</v>
@@ -487,37 +487,212 @@
         <v>Transferencia</v>
       </c>
       <c r="E3" t="str">
-        <v>aaa</v>
+        <v>Manu</v>
       </c>
       <c r="F3" t="str">
         <v>595971224560</v>
       </c>
       <c r="G3" t="str">
-        <v>8/2/2025, 19:04:09</v>
+        <v>8/2/2025, 19:32:29</v>
       </c>
       <c r="H3" t="str">
         <v>Terminado</v>
       </c>
       <c r="I3" t="str">
-        <v>8/2/2025, 19:04:51</v>
+        <v/>
       </c>
       <c r="J3" t="str">
-        <v>8/2/2025, 19:04:54</v>
+        <v>8/2/2025, 19:35:07</v>
       </c>
       <c r="K3" t="str">
-        <v>Nico</v>
+        <v>Marcos</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1739054074695</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Caipirinha</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1 litro(s)</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Transferencia</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Chiqui Falcon</v>
+      </c>
+      <c r="F4" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G4" t="str">
+        <v>8/2/2025, 19:34:43</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Pendiente</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v>Pame</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1739054236935</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Caipiruva</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2 litro(s)</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Efectivo</v>
+      </c>
+      <c r="E5" t="str">
+        <v>gei</v>
+      </c>
+      <c r="F5" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G5" t="str">
+        <v>8/2/2025, 19:37:18</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Pendiente</v>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v>Pame</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1739054255630</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Caipiruva</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1 litro(s)</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Transferencia</v>
+      </c>
+      <c r="E6" t="str">
+        <v>manu</v>
+      </c>
+      <c r="F6" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G6" t="str">
+        <v>8/2/2025, 19:37:41</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Pendiente</v>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v>Pame</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1739054326879</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Caipirinha</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1 litro(s)</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Transferencia</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Manuel Ayala</v>
+      </c>
+      <c r="F7" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G7" t="str">
+        <v>8/2/2025, 19:38:55</v>
+      </c>
+      <c r="H7" t="str">
+        <v>A Confirmar</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1739054446904</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Caipirinha</v>
+      </c>
+      <c r="C8" t="str">
+        <v>1 litro(s)</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Efectivo</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Manuel Ayala</v>
+      </c>
+      <c r="F8" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G8" t="str">
+        <v>8/2/2025, 19:40:57</v>
+      </c>
+      <c r="H8" t="str">
+        <v>A Confirmar</v>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -566,10 +741,21 @@
         <v>123456</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Pame</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregue usuarios por procesos y modificacion de tablas Usuarios y Pedidos
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -1,118 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\caipibar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95801237-9D85-43E4-948A-B9394DB08AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="20445" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Pedidos" sheetId="1" r:id="rId1"/>
+    <sheet name="Productos" sheetId="1" r:id="rId1"/>
     <sheet name="Usuarios" sheetId="2" r:id="rId2"/>
-    <sheet name="Productos" sheetId="3" r:id="rId3"/>
+    <sheet name="Pedidos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>ID Pedido</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Litros</t>
-  </si>
-  <si>
-    <t>Método de Pago</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Número de Cliente</t>
-  </si>
-  <si>
-    <t>Fecha Pedido</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Fecha Preparación</t>
-  </si>
-  <si>
-    <t>Fecha Terminado</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>nico</t>
-  </si>
-  <si>
-    <t>marcos</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>manu</t>
-  </si>
-  <si>
-    <t>pame</t>
-  </si>
-  <si>
-    <t>id_producto</t>
-  </si>
-  <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>caipirinha 1 litro(s)</t>
-  </si>
-  <si>
-    <t>caipirinha 2 litro(s)</t>
-  </si>
-  <si>
-    <t>caipiruva 1 litro(s)</t>
-  </si>
-  <si>
-    <t>caipiruva 2 litro(s)</t>
-  </si>
-  <si>
-    <t>caipiboom 1 litro(s)</t>
-  </si>
-  <si>
-    <t>caipiboom 2 litro(s)</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,21 +67,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -481,228 +398,286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id_producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>producto</v>
+      </c>
+      <c r="C1" t="str">
+        <v>precio</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="str">
+        <v>caipirinha 1 litro(s)</v>
+      </c>
+      <c r="C2">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="str">
+        <v>caipirinha 2 litro(s)</v>
+      </c>
+      <c r="C3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="str">
+        <v>caipiruva 1 litro(s)</v>
+      </c>
+      <c r="C4">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5" t="str">
+        <v>caipiruva 2 litro(s)</v>
+      </c>
+      <c r="C5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6" t="str">
+        <v>caipiboom 1 litro(s)</v>
+      </c>
+      <c r="C6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
+      <c r="B7" t="str">
+        <v>caipiboom 2 litro(s)</v>
+      </c>
+      <c r="C7">
+        <v>60000</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:L1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>username</v>
+      </c>
+      <c r="C1" t="str">
+        <v>password</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="str">
+        <v>cortar_macerar</v>
+      </c>
+      <c r="C2" t="str">
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="str">
+        <v>dosificar</v>
+      </c>
+      <c r="C3" t="str">
         <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="str">
+        <v>coctelera</v>
+      </c>
+      <c r="C4" t="str">
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="str">
+        <v>garnish</v>
+      </c>
+      <c r="C5" t="str">
         <v>123456</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>pamela</v>
+      </c>
+      <c r="C6" t="str">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C5" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID Pedido</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Litros</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Método de Pago</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Nombre</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Número de Cliente</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Fecha Pedido</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Estado</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Fecha A Confirmar</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Fecha Cortar/Macerar</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Fecha Dosificar</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Fecha Coctelera</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Fecha Garnish</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Fecha Terminado</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Usuario</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Precio</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1739146767021</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Caipirinha</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2 litro(s)</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Efectivo</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Manue Ayala</v>
+      </c>
+      <c r="F2" t="str">
+        <v>595971224560</v>
+      </c>
+      <c r="G2" t="str">
+        <v>9/2/2025, 21:19:37</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Terminado</v>
+      </c>
+      <c r="I2" t="str">
+        <v>9/2/2025, 21:19:37</v>
+      </c>
+      <c r="J2" t="str">
+        <v>9/2/2025, 21:19:42</v>
+      </c>
+      <c r="K2" t="str">
+        <v>9/2/2025, 21:19:46</v>
+      </c>
+      <c r="L2" t="str">
+        <v>9/2/2025, 21:19:48</v>
+      </c>
+      <c r="M2" t="str">
+        <v>9/2/2025, 21:19:52</v>
+      </c>
+      <c r="N2" t="str">
+        <v>9/2/2025, 21:19:55</v>
+      </c>
+      <c r="O2" t="str">
+        <v>garnish</v>
+      </c>
+      <c r="P2">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7">
-        <v>60000</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C7" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>